<commit_message>
Re-run the 2 datasets after finding the best embedding size
</commit_message>
<xml_diff>
--- a/results/MHD/model_results.xlsx
+++ b/results/MHD/model_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>MSE</t>
+          <t>RMSE</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>MSE_log</t>
         </is>
       </c>
     </row>
@@ -467,16 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8635341292596914</v>
+        <v>0.775719984354989</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3540730117506894</v>
+        <v>0.1784170197730449</v>
       </c>
       <c r="D2" t="n">
-        <v>0.78</v>
+        <v>0.806</v>
       </c>
       <c r="E2" t="n">
-        <v>4.822111486028375e+18</v>
+        <v>2232917813.31779</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0112439613306092</v>
       </c>
     </row>
     <row r="3">
@@ -486,16 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8630532496886421</v>
+        <v>0.803511885674746</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3602315458874696</v>
+        <v>0.1689024077359783</v>
       </c>
       <c r="D3" t="n">
-        <v>0.784</v>
+        <v>0.79</v>
       </c>
       <c r="E3" t="n">
-        <v>4.839103682614772e+18</v>
+        <v>2089996659.117547</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.009878683005223553</v>
       </c>
     </row>
     <row r="4">
@@ -505,16 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6919142892318983</v>
+        <v>0.6447146954908073</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6384143333807547</v>
+        <v>0.3189993446933566</v>
       </c>
       <c r="D4" t="n">
-        <v>0.452</v>
+        <v>0.574</v>
       </c>
       <c r="E4" t="n">
-        <v>1.088641164649281e+19</v>
+        <v>2810386636.278114</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.03115809645376205</v>
       </c>
     </row>
     <row r="5">
@@ -524,16 +538,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6947083994051351</v>
+        <v>0.6444440888307548</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6073426258069087</v>
+        <v>0.3190082859223518</v>
       </c>
       <c r="D5" t="n">
-        <v>0.464</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="E5" t="n">
-        <v>1.078767992194878e+19</v>
+        <v>2811456712.318631</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.02986115581908628</v>
       </c>
     </row>
     <row r="6">
@@ -543,16 +560,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8660150897891783</v>
+        <v>0.8181890743697067</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3877035484512394</v>
+        <v>0.1721062464955148</v>
       </c>
       <c r="D6" t="n">
-        <v>0.748</v>
+        <v>0.804</v>
       </c>
       <c r="E6" t="n">
-        <v>4.734445110540337e+18</v>
+        <v>2010422973.744161</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.01033476672484333</v>
       </c>
     </row>
     <row r="7">
@@ -562,16 +582,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8669716588428347</v>
+        <v>0.8090055490035011</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3909966662245142</v>
+        <v>0.1695272787264475</v>
       </c>
       <c r="D7" t="n">
-        <v>0.75</v>
+        <v>0.798</v>
       </c>
       <c r="E7" t="n">
-        <v>4.700644112563388e+18</v>
+        <v>2060572143.494536</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.009944598743791801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run MHD for r = 50
</commit_message>
<xml_diff>
--- a/results/MHD/model_results.xlsx
+++ b/results/MHD/model_results.xlsx
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.803511885674746</v>
+        <v>0.8063704052585373</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1689024077359783</v>
+        <v>0.1662004957965591</v>
       </c>
       <c r="D3" t="n">
-        <v>0.79</v>
+        <v>0.8139999999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>2089996659.117547</v>
+        <v>2074738269.309195</v>
       </c>
       <c r="F3" t="n">
-        <v>0.009878683005223553</v>
+        <v>0.009928829375639398</v>
       </c>
     </row>
     <row r="4">
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6444440888307548</v>
+        <v>0.6424436849792784</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3190082859223518</v>
+        <v>0.3201680102268146</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5659999999999999</v>
+        <v>0.574</v>
       </c>
       <c r="E5" t="n">
-        <v>2811456712.318631</v>
+        <v>2819354430.266713</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02986115581908628</v>
+        <v>0.03448963229494235</v>
       </c>
     </row>
     <row r="6">
@@ -582,19 +582,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8090055490035011</v>
+        <v>0.8233898036780043</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1695272787264475</v>
+        <v>0.1640556571329358</v>
       </c>
       <c r="D7" t="n">
-        <v>0.798</v>
+        <v>0.802</v>
       </c>
       <c r="E7" t="n">
-        <v>2060572143.494536</v>
+        <v>1981460121.101597</v>
       </c>
       <c r="F7" t="n">
-        <v>0.009944598743791801</v>
+        <v>0.00955756944128665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>